<commit_message>
ege vedomosti: trash edition
</commit_message>
<xml_diff>
--- a/ege_vedomosti/template.xlsx
+++ b/ege_vedomosti/template.xlsx
@@ -72,9 +72,6 @@
     <t>М.П.</t>
   </si>
   <si>
-    <t>Дата выдачи «______»__________________ ______ г. регистрационный №______________________</t>
-  </si>
-  <si>
     <t>документ, удостоверяющий личность: &lt;template: pasport_data&gt;</t>
   </si>
   <si>
@@ -97,13 +94,35 @@
   </si>
   <si>
     <t>&lt;template: employee2_fio&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Дата выдачи </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>&lt;template: date&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> регистрационный №______________________</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -131,6 +150,19 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -198,36 +230,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -235,7 +238,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -522,8 +557,8 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -540,111 +575,111 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="A6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="A8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:9" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12" t="s">
+      <c r="F13" s="20"/>
+      <c r="G13" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="12"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -735,171 +770,186 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
+      <c r="A28" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
     </row>
     <row r="29" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="21"/>
+      <c r="A32" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="15"/>
       <c r="D32" s="1"/>
-      <c r="F32" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
+      <c r="F32" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="13"/>
       <c r="D33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
     </row>
     <row r="37" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="D37" s="1"/>
+      <c r="F37" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="D37" s="1"/>
-      <c r="F37" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="24"/>
+      <c r="B38" s="13"/>
       <c r="D38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
     </row>
     <row r="39" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="22"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
+      <c r="A45" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F32:I32"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="A45:I45"/>
     <mergeCell ref="A33:B33"/>
@@ -909,21 +959,6 @@
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="F38:I38"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <pageMargins left="0.39370078740157477" right="0.39370078740157477" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>

</xml_diff>